<commit_message>
Added my query ideas and progress!
12 query ideas
</commit_message>
<xml_diff>
--- a/Data Dictionary & Project Work Flow.xlsx
+++ b/Data Dictionary & Project Work Flow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayot\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\UIowa Fall 2018\Database Management &amp; Data Visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A28621E6-DABF-4212-8F8B-9FFBAA069574}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AAB86A61-4C03-4E9D-B711-8C2C2CE5E66B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="95">
   <si>
     <t>ProjectID</t>
   </si>
@@ -269,6 +269,51 @@
   </si>
   <si>
     <t>DERIVED</t>
+  </si>
+  <si>
+    <t>Nauman, O</t>
+  </si>
+  <si>
+    <t>Not Queried</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Which countries have had the highest % of successful kickstarter projects?</t>
+  </si>
+  <si>
+    <t>Which Main Category has had the highest % of successful projects?</t>
+  </si>
+  <si>
+    <t>Which Sub Category within this has had the highest % of successful projects?</t>
+  </si>
+  <si>
+    <t>Which Kickstarter has raised the most $?</t>
+  </si>
+  <si>
+    <t>Which Kickstarter has raised the most $ per backer?</t>
+  </si>
+  <si>
+    <t>Avg kickstarter $ raised per year</t>
+  </si>
+  <si>
+    <t>Avg kickstarter $ raised per month</t>
+  </si>
+  <si>
+    <t>Avg goal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% of projects raising $0 </t>
+  </si>
+  <si>
+    <t>Just an idea to play with: I think it would be cool to do something with the %Like% function in the title but am unsure of what would make the most sense? Maybe like something sad or dramatic?</t>
+  </si>
+  <si>
+    <t>Avg $ raised per country</t>
+  </si>
+  <si>
+    <t>Number of campaigns per year</t>
   </si>
 </sst>
 </file>
@@ -667,23 +712,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -694,7 +739,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -702,7 +747,7 @@
         <v>1234567</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -710,7 +755,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -718,7 +763,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -726,7 +771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -734,7 +779,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -742,7 +787,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -750,7 +795,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -761,7 +806,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -769,7 +814,7 @@
         <v>1234.56</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -777,7 +822,7 @@
         <v>1234.45</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -788,7 +833,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -796,7 +841,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -804,12 +849,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -817,7 +862,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -825,7 +870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -833,12 +878,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -846,7 +891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>2</v>
       </c>
@@ -854,7 +899,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -862,7 +907,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -870,12 +915,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -883,7 +928,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>16</v>
       </c>
@@ -891,7 +936,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -899,7 +944,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -907,7 +952,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -915,7 +960,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -923,7 +968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -941,33 +986,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.296875" customWidth="1"/>
-    <col min="3" max="3" width="65.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.9140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="56.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="59.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.69921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -1020,7 +1065,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1073,7 +1118,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1124,7 +1169,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -1175,7 +1220,16 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
       <c r="D5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1184,157 +1238,256 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
       <c r="D6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
       <c r="D7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
+        <v>86</v>
+      </c>
       <c r="D8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
       <c r="D9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
       <c r="D10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
       <c r="D11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
       <c r="D12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" t="s">
+        <v>91</v>
+      </c>
       <c r="D13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
       <c r="D14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
       <c r="D15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
       <c r="D16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D31">
         <f>D30+1</f>
         <v>30</v>

</xml_diff>